<commit_message>
new jobs and cleaning up old ones.
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\renato\ppt-doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF66A97-549B-4D1A-ACC7-79AE3898CD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02D9657-0E30-4320-BA18-A582A8E62375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2265" yWindow="2505" windowWidth="21600" windowHeight="11295" xr2:uid="{E2EAAA9B-09FC-4773-92F8-622FD93420C8}"/>
+    <workbookView xWindow="30555" yWindow="1350" windowWidth="21600" windowHeight="11295" xr2:uid="{E2EAAA9B-09FC-4773-92F8-622FD93420C8}"/>
   </bookViews>
   <sheets>
     <sheet name="DRE Saida" sheetId="1" r:id="rId1"/>
+    <sheet name="Margem Financeira" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>Labels</t>
   </si>
@@ -78,13 +79,19 @@
   </si>
   <si>
     <t>9M25</t>
+  </si>
+  <si>
+    <t>teste feito</t>
+  </si>
+  <si>
+    <t>teste 2 feito</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +106,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -121,9 +134,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{417E299C-E79D-4FD4-B55D-DB1E7B3327CE}">
-  <dimension ref="B3:N21"/>
+  <dimension ref="B3:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,8 +597,103 @@
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="L21" s="1"/>
     </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB80353-2AEA-4B03-BD7E-AB8ECF39D507}">
+  <dimension ref="W3:AK9"/>
+  <sheetViews>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="23:37" x14ac:dyDescent="0.25">
+      <c r="W3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="23:37" x14ac:dyDescent="0.25">
+      <c r="W9">
+        <v>9.9</v>
+      </c>
+      <c r="X9">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="Y9">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="Z9">
+        <v>9.6</v>
+      </c>
+      <c r="AA9">
+        <v>9.9</v>
+      </c>
+      <c r="AB9">
+        <v>11.1</v>
+      </c>
+      <c r="AC9">
+        <v>9.9</v>
+      </c>
+      <c r="AD9">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="AE9">
+        <v>9.5</v>
+      </c>
+      <c r="AJ9">
+        <v>9.6</v>
+      </c>
+      <c r="AK9">
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new graphs and updated scripts for data vis
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\renato\ppt-doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4536068E-D06F-4AD0-97B3-55F911781CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079B376D-3A47-492A-B13B-669C0015D6DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="1515" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{E2EAAA9B-09FC-4773-92F8-622FD93420C8}"/>
+    <workbookView xWindow="2130" yWindow="1860" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{E2EAAA9B-09FC-4773-92F8-622FD93420C8}"/>
   </bookViews>
   <sheets>
     <sheet name="DRE Saida" sheetId="1" r:id="rId1"/>
     <sheet name="Qualidade Cart 2682" sheetId="3" r:id="rId2"/>
-    <sheet name="Margem Financeira" sheetId="2" r:id="rId3"/>
+    <sheet name="Emprestimos" sheetId="4" r:id="rId3"/>
+    <sheet name="Seguros e Cartoes" sheetId="5" r:id="rId4"/>
+    <sheet name="Margem Financeira" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>Labels</t>
   </si>
@@ -98,6 +100,21 @@
   </si>
   <si>
     <t>Atacado</t>
+  </si>
+  <si>
+    <t>Demais</t>
+  </si>
+  <si>
+    <t>Placas Solares</t>
+  </si>
+  <si>
+    <t>Consignado Privado</t>
+  </si>
+  <si>
+    <t>EGV</t>
+  </si>
+  <si>
+    <t>Cartoes</t>
   </si>
 </sst>
 </file>
@@ -630,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B4CFF7-3A85-4820-951F-62E41E9FBB53}">
   <dimension ref="B7:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,6 +847,145 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E23628D-2121-49A9-92D5-277D45F162FD}">
+  <dimension ref="C4:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="E5">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="F5">
+        <v>9.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>4.2649999999999997</v>
+      </c>
+      <c r="E6">
+        <v>3.9140000000000001</v>
+      </c>
+      <c r="F6">
+        <v>3.7949999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="E7">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="F7">
+        <v>0.39500000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>3.83</v>
+      </c>
+      <c r="E8">
+        <v>4.5119999999999996</v>
+      </c>
+      <c r="F8">
+        <v>4.7969999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>8.76</v>
+      </c>
+      <c r="E9">
+        <v>9.0030000000000001</v>
+      </c>
+      <c r="F9">
+        <v>9.08</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F3A3B47-E08A-478E-9E32-E383F8DD5BE7}">
+  <dimension ref="C14:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>4.5419999999999998</v>
+      </c>
+      <c r="E15">
+        <v>4.8109999999999999</v>
+      </c>
+      <c r="F15">
+        <v>4.8289999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB80353-2AEA-4B03-BD7E-AB8ECF39D507}">
   <dimension ref="W3:AK9"/>
   <sheetViews>

</xml_diff>

<commit_message>
new fields for variation
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\renato\ppt-doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079B376D-3A47-492A-B13B-669C0015D6DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA344D4-5ACE-464F-9521-9B3342BF2B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="1860" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{E2EAAA9B-09FC-4773-92F8-622FD93420C8}"/>
+    <workbookView xWindow="2475" yWindow="2205" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{E2EAAA9B-09FC-4773-92F8-622FD93420C8}"/>
   </bookViews>
   <sheets>
     <sheet name="DRE Saida" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>Labels</t>
   </si>
@@ -115,13 +115,22 @@
   </si>
   <si>
     <t>Cartoes</t>
+  </si>
+  <si>
+    <t>3T25/2T25</t>
+  </si>
+  <si>
+    <t>3T25/3T24</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +152,13 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -161,18 +177,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -848,15 +867,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E23628D-2121-49A9-92D5-277D45F162FD}">
-  <dimension ref="C4:F9"/>
+  <dimension ref="C4:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>5</v>
       </c>
@@ -866,8 +888,14 @@
       <c r="F4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>19</v>
       </c>
@@ -880,8 +908,14 @@
       <c r="F5">
         <v>9.2999999999999999E-2</v>
       </c>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="3">
+        <v>0.223</v>
+      </c>
+      <c r="H5" s="3">
+        <v>-0.33400000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>20</v>
       </c>
@@ -894,8 +928,14 @@
       <c r="F6">
         <v>3.7949999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="3">
+        <v>-0.03</v>
+      </c>
+      <c r="H6" s="3">
+        <v>-0.11</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>21</v>
       </c>
@@ -908,8 +948,14 @@
       <c r="F7">
         <v>0.39500000000000002</v>
       </c>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="3">
+        <v>-0.13600000000000001</v>
+      </c>
+      <c r="H7" s="3">
+        <v>-0.248</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>22</v>
       </c>
@@ -922,8 +968,14 @@
       <c r="F8">
         <v>4.7969999999999997</v>
       </c>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="3">
+        <v>6.3E-2</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.253</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>15</v>
       </c>
@@ -935,6 +987,20 @@
       </c>
       <c r="F9">
         <v>9.08</v>
+      </c>
+      <c r="G9" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="H9" s="3">
+        <v>3.6999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="3">
+        <v>-0.154</v>
+      </c>
+      <c r="H10" s="3">
+        <v>-0.26600000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -946,7 +1012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F3A3B47-E08A-478E-9E32-E383F8DD5BE7}">
   <dimension ref="C14:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
handler for charts_common tests
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\renato\ppt-doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA344D4-5ACE-464F-9521-9B3342BF2B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C873FD-A93B-4785-AEF3-2197DACD5A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2475" yWindow="2205" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{E2EAAA9B-09FC-4773-92F8-622FD93420C8}"/>
+    <workbookView xWindow="2820" yWindow="2550" windowWidth="21600" windowHeight="11295" xr2:uid="{E2EAAA9B-09FC-4773-92F8-622FD93420C8}"/>
   </bookViews>
   <sheets>
     <sheet name="DRE Saida" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
   <si>
     <t>Labels</t>
   </si>
@@ -121,6 +121,33 @@
   </si>
   <si>
     <t>3T25/3T24</t>
+  </si>
+  <si>
+    <t>9%</t>
+  </si>
+  <si>
+    <t>9,4%</t>
+  </si>
+  <si>
+    <t>10%</t>
+  </si>
+  <si>
+    <t>11,1%</t>
+  </si>
+  <si>
+    <t>15%</t>
+  </si>
+  <si>
+    <t>16%</t>
+  </si>
+  <si>
+    <t>15,1%</t>
+  </si>
+  <si>
+    <t>12,1%</t>
+  </si>
+  <si>
+    <t>15,4%</t>
   </si>
 </sst>
 </file>
@@ -181,13 +208,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{417E299C-E79D-4FD4-B55D-DB1E7B3327CE}">
   <dimension ref="B3:N36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,42 +639,77 @@
       <c r="N18" s="1"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C20">
-        <v>9</v>
-      </c>
-      <c r="D20">
-        <v>9.4</v>
-      </c>
-      <c r="E20">
-        <v>10</v>
-      </c>
-      <c r="F20">
-        <v>11.1</v>
-      </c>
-      <c r="G20">
-        <v>15</v>
-      </c>
-      <c r="H20">
-        <v>16</v>
-      </c>
-      <c r="I20">
-        <v>16</v>
-      </c>
-      <c r="J20">
-        <v>15.1</v>
-      </c>
-      <c r="K20">
-        <v>15</v>
-      </c>
-      <c r="L20">
-        <v>12.1</v>
-      </c>
-      <c r="M20">
-        <v>15.4</v>
+      <c r="C20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="L21" s="1"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C25" s="4">
+        <v>0.09</v>
+      </c>
+      <c r="D25" s="5">
+        <v>9.4E-2</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0.111</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="I25" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="J25" s="5">
+        <v>0.151</v>
+      </c>
+      <c r="K25" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="L25" s="5">
+        <v>0.121</v>
+      </c>
+      <c r="M25" s="5">
+        <v>0.154</v>
+      </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
@@ -869,7 +934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E23628D-2121-49A9-92D5-277D45F162FD}">
   <dimension ref="C4:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
New Donut Charts and Others
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\renato\ppt-doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C873FD-A93B-4785-AEF3-2197DACD5A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F8C8DE-F3BE-4E7B-8C20-DB056B9A3189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="2550" windowWidth="21600" windowHeight="11295" xr2:uid="{E2EAAA9B-09FC-4773-92F8-622FD93420C8}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{E2EAAA9B-09FC-4773-92F8-622FD93420C8}"/>
   </bookViews>
   <sheets>
     <sheet name="DRE Saida" sheetId="1" r:id="rId1"/>
-    <sheet name="Qualidade Cart 2682" sheetId="3" r:id="rId2"/>
-    <sheet name="Emprestimos" sheetId="4" r:id="rId3"/>
-    <sheet name="Seguros e Cartoes" sheetId="5" r:id="rId4"/>
-    <sheet name="Margem Financeira" sheetId="2" r:id="rId5"/>
+    <sheet name="Pizza Teste" sheetId="6" r:id="rId2"/>
+    <sheet name="Qualidade Cart 2682" sheetId="3" r:id="rId3"/>
+    <sheet name="Emprestimos" sheetId="4" r:id="rId4"/>
+    <sheet name="Seguros e Cartoes" sheetId="5" r:id="rId5"/>
+    <sheet name="Margem Financeira" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="50">
   <si>
     <t>Labels</t>
   </si>
@@ -148,6 +149,51 @@
   </si>
   <si>
     <t>15,4%</t>
+  </si>
+  <si>
+    <t>Carteira de Crédito</t>
+  </si>
+  <si>
+    <t>Veiculos Leves</t>
+  </si>
+  <si>
+    <t>Growth</t>
+  </si>
+  <si>
+    <t>Veiculos Leves Usados</t>
+  </si>
+  <si>
+    <t>Corporate</t>
+  </si>
+  <si>
+    <t>Large e Instituições Financeiras</t>
+  </si>
+  <si>
+    <t>PME</t>
+  </si>
+  <si>
+    <t>Cartões</t>
+  </si>
+  <si>
+    <t>Painéis Solares</t>
+  </si>
+  <si>
+    <t>Motos, Pesados e Novos</t>
+  </si>
+  <si>
+    <t>Porcentagem</t>
+  </si>
+  <si>
+    <t>Valor(bi)</t>
+  </si>
+  <si>
+    <t>Receitas de Serviços</t>
+  </si>
+  <si>
+    <t>Variacoes</t>
+  </si>
+  <si>
+    <t>Destaques do Trimestre</t>
   </si>
 </sst>
 </file>
@@ -208,7 +254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -218,6 +264,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,7 +602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{417E299C-E79D-4FD4-B55D-DB1E7B3327CE}">
   <dimension ref="B3:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
@@ -728,6 +775,1870 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44452379-0FE0-41DB-BDE4-79B6F1D7D785}">
+  <dimension ref="A1:N285"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2">
+        <v>44.495999999999995</v>
+      </c>
+      <c r="D2" s="7">
+        <f>C2/SUM($C$2:$C$1048576)</f>
+        <v>0.47999999999999987</v>
+      </c>
+      <c r="N2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3">
+        <v>13.904999999999998</v>
+      </c>
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D66" si="0">C3/SUM($C$2:$C$1048576)</f>
+        <v>0.14999999999999994</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="3">
+        <v>-0.13300000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>10.196999999999999</v>
+      </c>
+      <c r="D4" s="7">
+        <f t="shared" si="0"/>
+        <v>0.10999999999999997</v>
+      </c>
+      <c r="H4">
+        <v>685</v>
+      </c>
+      <c r="I4">
+        <v>556</v>
+      </c>
+      <c r="J4">
+        <v>624</v>
+      </c>
+      <c r="K4">
+        <v>1984</v>
+      </c>
+      <c r="L4">
+        <v>1798</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>0.92699999999999994</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999967E-3</v>
+      </c>
+      <c r="N5" s="3">
+        <v>-0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6">
+        <v>2.7809999999999997</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>2.9999999999999992E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7">
+        <v>4.6349999999999998</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>4.9999999999999989E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8">
+        <v>4.6349999999999998</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>4.9999999999999989E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9">
+        <v>3.7079999999999997</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>3.9999999999999987E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10">
+        <v>7.4159999999999995</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
+        <v>7.9999999999999974E-2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D12" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D13" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D14" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D15" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D16" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D54" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D64" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" s="7">
+        <f t="shared" ref="D67:D130" si="1">C67/SUM($C$2:$C$1048576)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D69" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D70" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D71" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D72" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D73" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D74" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D75" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D76" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D77" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D78" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D79" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D80" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D82" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D85" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D86" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D87" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D88" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D89" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D90" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D91" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D92" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D93" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D94" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D95" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D96" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D97" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D98" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D99" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D100" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D101" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D102" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D103" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D104" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D105" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D106" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D107" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D108" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D109" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D110" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D111" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D112" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D113" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D114" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D115" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D116" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D117" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D118" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D119" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D120" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D121" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D122" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D123" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D124" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D125" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D126" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D127" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D128" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D129" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D130" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D131" s="7">
+        <f t="shared" ref="D131:D194" si="2">C131/SUM($C$2:$C$1048576)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D132" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D133" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D134" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D135" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D136" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D137" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D138" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D139" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D140" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D141" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D142" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D143" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D144" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D145" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D146" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D147" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D148" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D149" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D150" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D151" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D152" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D153" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D154" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D155" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D156" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D157" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D158" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D159" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D160" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D161" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D162" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D163" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D164" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D165" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D166" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D167" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D168" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D169" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D170" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D171" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D172" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D173" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D174" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D175" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D176" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D177" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D178" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D179" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D180" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D181" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D182" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D183" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D184" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D185" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D186" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D187" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D188" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D189" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D190" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D191" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D192" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D193" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D194" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D195" s="7">
+        <f t="shared" ref="D195:D258" si="3">C195/SUM($C$2:$C$1048576)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D196" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D197" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D198" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D199" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D200" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D201" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D202" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D203" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D204" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D205" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D206" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D207" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D208" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D209" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D210" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D211" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D212" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D213" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D214" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D215" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D216" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D217" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D218" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D219" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D220" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D221" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D222" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D223" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D224" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D225" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D226" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D227" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D228" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D229" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D230" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D231" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D232" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D233" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D234" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D235" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D236" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D237" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D238" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D239" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D240" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D241" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D242" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D243" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D244" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D245" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D246" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D247" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D248" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D249" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D250" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D251" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D252" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D253" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D254" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D255" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D256" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D257" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D258" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D259" s="7">
+        <f t="shared" ref="D259:D285" si="4">C259/SUM($C$2:$C$1048576)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D260" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D261" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D262" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D263" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D264" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D265" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D266" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D267" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D268" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D269" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D270" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D271" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D272" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D273" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D274" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D275" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D276" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D277" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D278" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D279" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D280" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D281" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D282" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D283" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D284" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D285" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B4CFF7-3A85-4820-951F-62E41E9FBB53}">
   <dimension ref="B7:P10"/>
   <sheetViews>
@@ -930,7 +2841,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E23628D-2121-49A9-92D5-277D45F162FD}">
   <dimension ref="C4:H10"/>
   <sheetViews>
@@ -1073,7 +2984,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F3A3B47-E08A-478E-9E32-E383F8DD5BE7}">
   <dimension ref="C14:F15"/>
   <sheetViews>
@@ -1116,7 +3027,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB80353-2AEA-4B03-BD7E-AB8ECF39D507}">
   <dimension ref="W3:AK9"/>
   <sheetViews>

</xml_diff>